<commit_message>
update ontologies and vocabolaries
</commit_message>
<xml_diff>
--- a/ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
+++ b/ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-public-services/channel/channel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="150">
   <si>
     <t>01</t>
   </si>
@@ -63,21 +63,12 @@
     <t>02</t>
   </si>
   <si>
-    <t>Sito Web</t>
-  </si>
-  <si>
     <t>02.1</t>
   </si>
   <si>
-    <t>Modulo online libero</t>
-  </si>
-  <si>
     <t>02.2</t>
   </si>
   <si>
-    <t>Modulo online precompilato</t>
-  </si>
-  <si>
     <t>03</t>
   </si>
   <si>
@@ -291,21 +282,9 @@
     <t>Sonstiger Vermittler</t>
   </si>
   <si>
-    <t>Web Site</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Free Online Form</t>
-  </si>
-  <si>
     <t>Online-Formular nicht ausgefüllt</t>
   </si>
   <si>
-    <t>Pre-filled Online Form</t>
-  </si>
-  <si>
     <t>Vorkompiliertes Online-Modul</t>
   </si>
   <si>
@@ -469,6 +448,27 @@
   </si>
   <si>
     <t>label_DEU_3_livello</t>
+  </si>
+  <si>
+    <t>Applicativo</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Applikation</t>
+  </si>
+  <si>
+    <t>Applicazione con compilazione modulo libero</t>
+  </si>
+  <si>
+    <t>Applicazione con modulo precompilato</t>
+  </si>
+  <si>
+    <t>Application with pre-filled form</t>
+  </si>
+  <si>
+    <t>Application with free form</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -610,7 +614,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -635,6 +639,8 @@
     <cellStyle name="Collegamento ipertestuale" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -659,6 +665,8 @@
     <cellStyle name="Collegamento visitato" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -988,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1012,40 +1020,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1056,34 +1064,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1094,34 +1102,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1132,34 +1140,34 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1170,34 +1178,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1208,34 +1216,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1246,34 +1254,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1284,22 +1292,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>10</v>
@@ -1308,10 +1316,10 @@
         <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1322,34 +1330,34 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1357,25 +1365,25 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L10" s="8"/>
     </row>
@@ -1384,634 +1392,667 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="7"/>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" t="s">
-        <v>100</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="7"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="7"/>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>103</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="J15" s="1"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="H17" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="L17" s="8"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="H18" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>105</v>
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" t="s">
-        <v>110</v>
+        <v>29</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="F21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>113</v>
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" t="s">
-        <v>115</v>
-      </c>
-      <c r="K21" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>117</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>113</v>
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
       </c>
       <c r="H22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" t="s">
-        <v>118</v>
-      </c>
-      <c r="K22" t="s">
-        <v>119</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>120</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" t="s">
-        <v>121</v>
-      </c>
-      <c r="K23" t="s">
-        <v>122</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>123</v>
-      </c>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>125</v>
+      <c r="H24" t="s">
+        <v>107</v>
       </c>
       <c r="I24" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J24" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="K24" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>51</v>
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" t="s">
+        <v>43</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="K25" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>52</v>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>44</v>
       </c>
       <c r="J26" t="s">
-        <v>53</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
+      </c>
+      <c r="K26" t="s">
+        <v>115</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>54</v>
+        <v>118</v>
+      </c>
+      <c r="I27" t="s">
+        <v>47</v>
       </c>
       <c r="J27" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="K27" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="J28" t="s">
+        <v>122</v>
+      </c>
+      <c r="K28" t="s">
+        <v>123</v>
+      </c>
+      <c r="L28" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" t="s">
-        <v>57</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="J29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J29" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L29" s="9" t="s">
-        <v>59</v>
+      <c r="L29" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5"/>
@@ -2022,17 +2063,38 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="3"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="5"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>